<commit_message>
added test for invalid credentials and added functionality for reading excel tables
</commit_message>
<xml_diff>
--- a/src/main/java/resources/credentials.xlsx
+++ b/src/main/java/resources/credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\gitClone\test_automation_selenium_java_maven\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36C358BE-8DA1-4600-A40D-194A229B1670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429FBC47-6F57-418D-ACB5-9C1556332EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6B95E9A-A1C3-476D-80F9-2A352A50EE81}"/>
+    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{A6B95E9A-A1C3-476D-80F9-2A352A50EE81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Passwords</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>invalid@test.com</t>
+  </si>
+  <si>
+    <t>invalid!23</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -414,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CBF4DB-8A2F-4244-B866-D0ABD36DC719}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -450,11 +459,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{42C8C80C-D52E-4CE0-AF97-EB32CB6DC032}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5B3955FF-75BA-47C2-970E-3DC4795C4119}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>